<commit_message>
primeras notas de edición y outline.docx
</commit_message>
<xml_diff>
--- a/data/datos01_ciencia_tecnologia.xlsx
+++ b/data/datos01_ciencia_tecnologia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0. Pen DRive\0. CLM_en_datos\informe-2026\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D580F6-2E83-49CF-B1AC-F6059EFC916D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7270BD-D56F-4242-8A1A-30ACBA2234AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="996" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="1200" windowWidth="23040" windowHeight="12204" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,30 +193,9 @@
     <t>Personal que utiliza ordenadores conectados a Internet con fines empresariales</t>
   </si>
   <si>
-    <t>Empresas con sitio/página web**</t>
-  </si>
-  <si>
     <t>Empresas que disponen de conexión a Internet*</t>
   </si>
   <si>
-    <t>Empresas que permiten teletrabajo*</t>
-  </si>
-  <si>
-    <t>Empleados que teletrabajan regularmente*</t>
-  </si>
-  <si>
-    <t>Empresas que realizan analítica de datos internamente**</t>
-  </si>
-  <si>
-    <t>Empresas que compran servicios de cloud computing**</t>
-  </si>
-  <si>
-    <t>Empresas que emplean tecnologías de IA**</t>
-  </si>
-  <si>
-    <t>Empresas que emplean especialistas en TIC*</t>
-  </si>
-  <si>
     <t>32,8</t>
   </si>
   <si>
@@ -262,13 +241,34 @@
     <t>2,8</t>
   </si>
   <si>
-    <t>Empresas con mujeres especialistas TIC***</t>
-  </si>
-  <si>
-    <t>Personal especialista TIC****</t>
-  </si>
-  <si>
-    <t>Empresas que utilizan medios sociales**</t>
+    <t>Porcentaje de personal especialista TIC sobre el total de personal</t>
+  </si>
+  <si>
+    <t>Empleados que teletrabajan regularmente(i)</t>
+  </si>
+  <si>
+    <t>Empresas con sitio/página web(ii)</t>
+  </si>
+  <si>
+    <t>Empresas que permiten teletrabajo(i)</t>
+  </si>
+  <si>
+    <t>Empresas que utilizan medios sociales(ii)</t>
+  </si>
+  <si>
+    <t>Empresas que realizan analítica de datos internamente(ii)</t>
+  </si>
+  <si>
+    <t>Empresas que compran servicios de cloud computing(ii)</t>
+  </si>
+  <si>
+    <t>Empresas que emplean tecnologías de IA(ii)</t>
+  </si>
+  <si>
+    <t>Empresas que emplean especialistas en TIC(i)</t>
+  </si>
+  <si>
+    <t>Empresas con mujeres especialistas TIC(iii)</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E7EF02-5A22-4303-A4A7-1668F0D88F33}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F8DE72-8676-4540-BEE4-60F9C67A3EB3}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="44">
         <v>98.8</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B6" s="48">
         <v>5.95</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="45" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B7" s="46">
         <v>75.900000000000006</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="45" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B8" s="46">
         <v>24.12</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="45" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B9" s="46">
         <v>54.89</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B10" s="46">
         <v>21.23</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B11" s="46">
         <v>23.48</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="45" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B12" s="46">
         <v>7.63</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="49" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B13" s="50">
         <v>8.48</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="49" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B14" s="50">
         <v>45.92</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="49" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B15" s="50">
         <v>1.27</v>
@@ -1686,16 +1686,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>45</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1703,16 +1703,16 @@
         <v>42</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1720,16 +1720,16 @@
         <v>43</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E3" s="42" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1737,16 +1737,16 @@
         <v>44</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>